<commit_message>
add Race Bahrain to excel
</commit_message>
<xml_diff>
--- a/seasons_excel/Formel1_2019_WM_3.xlsx
+++ b/seasons_excel/Formel1_2019_WM_3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/timkeller/git_repos/TK5/F1-virtualWC/seasons_excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5443253-5C04-694F-824F-FA513ECD6BE6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AE39E71-9A29-C345-BB82-41C1BD7DD4C2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="67680" yWindow="-1340" windowWidth="35460" windowHeight="20160" xr2:uid="{15EF9A06-B4D9-F442-81AB-3E6205016DF9}"/>
+    <workbookView xWindow="29140" yWindow="-940" windowWidth="35460" windowHeight="20160" xr2:uid="{15EF9A06-B4D9-F442-81AB-3E6205016DF9}"/>
   </bookViews>
   <sheets>
     <sheet name="Fahrerwertung" sheetId="1" r:id="rId1"/>
@@ -492,64 +492,64 @@
               <c:strCache>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
-                  <c:v>Leclerc</c:v>
+                  <c:v>Paul </c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>Andi </c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>Leclerc</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Hamilton</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>Vettel</c:v>
                 </c:pt>
-                <c:pt idx="3">
-                  <c:v>Paul </c:v>
-                </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
+                  <c:v>Verstappen</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>Perez</c:v>
                 </c:pt>
-                <c:pt idx="5">
-                  <c:v>Hamilton</c:v>
-                </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>Sainz</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
+                  <c:v>Lorenz </c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>Albon </c:v>
                 </c:pt>
-                <c:pt idx="8">
-                  <c:v>Verstappen</c:v>
-                </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>Räikkönen</c:v>
                 </c:pt>
-                <c:pt idx="10">
-                  <c:v>Lorenz </c:v>
-                </c:pt>
                 <c:pt idx="11">
+                  <c:v>Tim </c:v>
+                </c:pt>
+                <c:pt idx="12">
                   <c:v>Gasly</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="13">
                   <c:v>Grosjean</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="14">
                   <c:v>Hülkenberg</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="15">
                   <c:v>Ricciardo</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="16">
                   <c:v>Giovinazzi</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="17">
                   <c:v>Russell</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="18">
                   <c:v>Kyvat</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="19">
                   <c:v>Kubica </c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>Tim </c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -561,40 +561,40 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
-                  <c:v>25</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>18</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>15</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="6">
                   <c:v>12</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="7">
                   <c:v>10</c:v>
                 </c:pt>
-                <c:pt idx="5">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>4</c:v>
                 </c:pt>
-                <c:pt idx="8">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>1</c:v>
                 </c:pt>
-                <c:pt idx="10">
-                  <c:v>0</c:v>
-                </c:pt>
                 <c:pt idx="11">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>0</c:v>
@@ -1001,7 +1001,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Leclerc</c:v>
+                  <c:v>Paul </c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1037,7 +1037,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>25</c:v>
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>26</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1096,6 +1099,9 @@
                 <c:pt idx="0">
                   <c:v>18</c:v>
                 </c:pt>
+                <c:pt idx="1">
+                  <c:v>18</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1115,7 +1121,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Paul </c:v>
+                  <c:v>Hamilton</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1151,7 +1157,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>12</c:v>
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>15</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1172,7 +1181,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Sainz</c:v>
+                  <c:v>Perez</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1214,7 +1223,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>6</c:v>
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1235,7 +1247,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Tim </c:v>
+                  <c:v>Kubica </c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1277,6 +1289,9 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -1645,7 +1660,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Leclerc</c:v>
+                  <c:v>Paul </c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1667,7 +1682,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>25</c:v>
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>26</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1709,6 +1727,9 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>18</c:v>
                 </c:pt>
               </c:numCache>
@@ -2087,7 +2108,7 @@
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>Leclerc</c:v>
+                  <c:v>Paul </c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>Andi </c:v>
@@ -2102,10 +2123,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>25</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>18</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2284,7 +2305,7 @@
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>Leclerc</c:v>
+                  <c:v>Paul </c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>Andi </c:v>
@@ -2299,10 +2320,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>25</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>18</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2664,67 +2685,67 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>25</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>25</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>25</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>25</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>25</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>25</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>25</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>25</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>25</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>25</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>25</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>25</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>25</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>25</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>25</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>25</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>25</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>25</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>25</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>25</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>25</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2843,64 +2864,64 @@
                   <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>18</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>18</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>18</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>18</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>18</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>18</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>18</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>18</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>18</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>18</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>18</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>18</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>18</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>18</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>18</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>18</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>18</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>18</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>18</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>18</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3016,67 +3037,67 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>15</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>15</c:v>
+                  <c:v>33</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>15</c:v>
+                  <c:v>33</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>15</c:v>
+                  <c:v>33</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>15</c:v>
+                  <c:v>33</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>15</c:v>
+                  <c:v>33</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>15</c:v>
+                  <c:v>33</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>15</c:v>
+                  <c:v>33</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>15</c:v>
+                  <c:v>33</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>15</c:v>
+                  <c:v>33</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>15</c:v>
+                  <c:v>33</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>15</c:v>
+                  <c:v>33</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>15</c:v>
+                  <c:v>33</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>15</c:v>
+                  <c:v>33</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>15</c:v>
+                  <c:v>33</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>15</c:v>
+                  <c:v>33</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>15</c:v>
+                  <c:v>33</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>15</c:v>
+                  <c:v>33</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>15</c:v>
+                  <c:v>33</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>15</c:v>
+                  <c:v>33</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>15</c:v>
+                  <c:v>33</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3192,67 +3213,67 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>12</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>12</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>12</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>12</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>12</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>12</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>12</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>12</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>12</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>12</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>12</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>12</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>12</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>12</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>12</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>12</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>12</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>12</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>12</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>12</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>12</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3368,67 +3389,67 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>10</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>10</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>10</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>10</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>10</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>10</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>10</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>10</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>10</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>10</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>10</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>10</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>10</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>10</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>10</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>10</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>10</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>10</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>10</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3544,67 +3565,67 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>8</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>8</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>8</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>8</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>8</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>8</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>8</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>8</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>8</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>8</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>8</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>8</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>8</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>8</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>8</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>8</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>8</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>8</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>8</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3722,67 +3743,67 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>6</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>6</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>6</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>6</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>6</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>6</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>6</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>6</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>6</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>6</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>6</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>6</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>6</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>6</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>6</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>6</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3900,67 +3921,67 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>4</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>4</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>4</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>4</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>4</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>4</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>4</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>4</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>4</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>4</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>4</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>4</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>4</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>4</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4078,67 +4099,67 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>3</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>3</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>3</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>3</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>3</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>3</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>3</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>3</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>3</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>3</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>3</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4256,67 +4277,67 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>1</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4434,67 +4455,67 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4615,64 +4636,64 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -10157,7 +10178,7 @@
   <dimension ref="A1:AF26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10253,18 +10274,18 @@
       </c>
     </row>
     <row r="4" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
-        <v>6</v>
+      <c r="A4" s="9" t="s">
+        <v>19</v>
       </c>
       <c r="B4">
-        <f t="shared" ref="B4:B23" si="0">SUM(C4:W4)</f>
-        <v>25</v>
+        <f>SUM(C4:W4)</f>
+        <v>38</v>
       </c>
       <c r="C4">
-        <v>25</v>
-      </c>
-      <c r="X4">
-        <v>3</v>
+        <v>12</v>
+      </c>
+      <c r="D4">
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:32" x14ac:dyDescent="0.2">
@@ -10272,38 +10293,44 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <f t="shared" si="0"/>
+        <f>SUM(C5:W5)</f>
+        <v>36</v>
+      </c>
+      <c r="C5">
         <v>18</v>
       </c>
-      <c r="C5">
+      <c r="D5">
         <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>59</v>
+        <v>6</v>
       </c>
       <c r="B6">
-        <f t="shared" si="0"/>
-        <v>15</v>
+        <f>SUM(C6:W6)</f>
+        <v>33</v>
       </c>
       <c r="C6">
-        <v>15</v>
-      </c>
-      <c r="X6">
-        <v>4</v>
+        <v>25</v>
+      </c>
+      <c r="D6">
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="A7" s="9" t="s">
-        <v>19</v>
+      <c r="A7" s="1" t="s">
+        <v>61</v>
       </c>
       <c r="B7">
-        <f t="shared" si="0"/>
-        <v>12</v>
+        <f>SUM(C7:W7)</f>
+        <v>23</v>
       </c>
       <c r="C7">
-        <v>12</v>
+        <v>8</v>
+      </c>
+      <c r="D7">
+        <v>15</v>
       </c>
       <c r="AD7">
         <v>1</v>
@@ -10316,15 +10343,18 @@
       </c>
     </row>
     <row r="8" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="A8" s="9" t="s">
-        <v>12</v>
+      <c r="A8" s="2" t="s">
+        <v>59</v>
       </c>
       <c r="B8">
-        <f t="shared" si="0"/>
-        <v>10</v>
+        <f>SUM(C8:W8)</f>
+        <v>21</v>
       </c>
       <c r="C8">
-        <v>10</v>
+        <v>15</v>
+      </c>
+      <c r="D8">
+        <v>6</v>
       </c>
       <c r="AE8" s="1" t="s">
         <v>61</v>
@@ -10334,18 +10364,18 @@
       </c>
     </row>
     <row r="9" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
-        <v>61</v>
+      <c r="A9" s="6" t="s">
+        <v>7</v>
       </c>
       <c r="B9">
-        <f t="shared" si="0"/>
-        <v>8</v>
+        <f>SUM(C9:W9)</f>
+        <v>15</v>
       </c>
       <c r="C9">
-        <v>8</v>
-      </c>
-      <c r="X9">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="D9">
+        <v>12</v>
       </c>
       <c r="AD9">
         <v>2</v>
@@ -10358,15 +10388,18 @@
       </c>
     </row>
     <row r="10" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="A10" s="3" t="s">
-        <v>60</v>
+      <c r="A10" s="9" t="s">
+        <v>12</v>
       </c>
       <c r="B10">
-        <f t="shared" si="0"/>
-        <v>6</v>
+        <f>SUM(C10:W10)</f>
+        <v>12</v>
       </c>
       <c r="C10">
-        <v>6</v>
+        <v>10</v>
+      </c>
+      <c r="D10">
+        <v>2</v>
       </c>
       <c r="AE10" s="2" t="s">
         <v>59</v>
@@ -10376,18 +10409,18 @@
       </c>
     </row>
     <row r="11" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="A11" s="6" t="s">
-        <v>15</v>
+      <c r="A11" s="3" t="s">
+        <v>60</v>
       </c>
       <c r="B11">
-        <f t="shared" si="0"/>
+        <f>SUM(C11:W11)</f>
+        <v>10</v>
+      </c>
+      <c r="C11">
+        <v>6</v>
+      </c>
+      <c r="D11">
         <v>4</v>
-      </c>
-      <c r="C11">
-        <v>4</v>
-      </c>
-      <c r="X11">
-        <v>6</v>
       </c>
       <c r="AD11">
         <v>3</v>
@@ -10400,18 +10433,18 @@
       </c>
     </row>
     <row r="12" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="A12" s="6" t="s">
-        <v>7</v>
+      <c r="A12" s="5" t="s">
+        <v>3</v>
       </c>
       <c r="B12">
-        <f t="shared" si="0"/>
-        <v>3</v>
+        <f>SUM(C12:W12)</f>
+        <v>10</v>
       </c>
       <c r="C12">
-        <v>3</v>
-      </c>
-      <c r="X12">
-        <v>5</v>
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>10</v>
       </c>
       <c r="AE12" s="6" t="s">
         <v>15</v>
@@ -10421,15 +10454,18 @@
       </c>
     </row>
     <row r="13" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="A13" s="8" t="s">
-        <v>13</v>
+      <c r="A13" s="6" t="s">
+        <v>15</v>
       </c>
       <c r="B13">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <f>SUM(C13:W13)</f>
+        <v>4</v>
       </c>
       <c r="C13">
-        <v>1</v>
+        <v>4</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
       </c>
       <c r="AD13">
         <v>4</v>
@@ -10442,14 +10478,17 @@
       </c>
     </row>
     <row r="14" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="A14" s="5" t="s">
-        <v>3</v>
+      <c r="A14" s="8" t="s">
+        <v>13</v>
       </c>
       <c r="B14">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>SUM(C14:W14)</f>
+        <v>1</v>
       </c>
       <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14">
         <v>0</v>
       </c>
       <c r="AE14" s="5" t="s">
@@ -10460,15 +10499,18 @@
       </c>
     </row>
     <row r="15" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="A15" s="7" t="s">
-        <v>8</v>
+      <c r="A15" s="1" t="s">
+        <v>2</v>
       </c>
       <c r="B15">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>SUM(C15:W15)</f>
+        <v>1</v>
       </c>
       <c r="C15">
         <v>0</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
       </c>
       <c r="AD15">
         <v>5</v>
@@ -10481,14 +10523,17 @@
       </c>
     </row>
     <row r="16" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="A16" s="5" t="s">
-        <v>10</v>
+      <c r="A16" s="7" t="s">
+        <v>8</v>
       </c>
       <c r="B16">
-        <f t="shared" si="0"/>
+        <f>SUM(C16:W16)</f>
         <v>0</v>
       </c>
       <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16">
         <v>0</v>
       </c>
       <c r="AE16" s="9" t="s">
@@ -10499,14 +10544,17 @@
       </c>
     </row>
     <row r="17" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="A17" s="4" t="s">
-        <v>57</v>
+      <c r="A17" s="5" t="s">
+        <v>10</v>
       </c>
       <c r="B17">
-        <f t="shared" si="0"/>
+        <f>SUM(C17:W17)</f>
         <v>0</v>
       </c>
       <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17">
         <v>0</v>
       </c>
       <c r="AD17">
@@ -10521,13 +10569,16 @@
     </row>
     <row r="18" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
-        <v>9</v>
+        <v>57</v>
       </c>
       <c r="B18">
-        <f t="shared" si="0"/>
+        <f>SUM(C18:W18)</f>
         <v>0</v>
       </c>
       <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="D18">
         <v>0</v>
       </c>
       <c r="AE18" s="3" t="s">
@@ -10538,14 +10589,17 @@
       </c>
     </row>
     <row r="19" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="A19" s="8" t="s">
-        <v>14</v>
+      <c r="A19" s="4" t="s">
+        <v>9</v>
       </c>
       <c r="B19">
-        <f t="shared" si="0"/>
+        <f>SUM(C19:W19)</f>
         <v>0</v>
       </c>
       <c r="C19">
+        <v>0</v>
+      </c>
+      <c r="D19">
         <v>0</v>
       </c>
       <c r="AD19">
@@ -10559,14 +10613,17 @@
       </c>
     </row>
     <row r="20" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>17</v>
+      <c r="A20" s="8" t="s">
+        <v>14</v>
       </c>
       <c r="B20">
-        <f t="shared" si="0"/>
+        <f>SUM(C20:W20)</f>
         <v>0</v>
       </c>
       <c r="C20">
+        <v>0</v>
+      </c>
+      <c r="D20">
         <v>0</v>
       </c>
       <c r="AE20" s="4" t="s">
@@ -10577,14 +10634,17 @@
       </c>
     </row>
     <row r="21" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="A21" s="7" t="s">
-        <v>18</v>
+      <c r="A21" t="s">
+        <v>17</v>
       </c>
       <c r="B21">
-        <f t="shared" si="0"/>
+        <f>SUM(C21:W21)</f>
         <v>0</v>
       </c>
       <c r="C21">
+        <v>0</v>
+      </c>
+      <c r="D21">
         <v>0</v>
       </c>
       <c r="AD21">
@@ -10598,14 +10658,17 @@
       </c>
     </row>
     <row r="22" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>16</v>
+      <c r="A22" s="7" t="s">
+        <v>18</v>
       </c>
       <c r="B22">
-        <f t="shared" si="0"/>
+        <f>SUM(C22:W22)</f>
         <v>0</v>
       </c>
       <c r="C22">
+        <v>0</v>
+      </c>
+      <c r="D22">
         <v>0</v>
       </c>
       <c r="AE22" s="8" t="s">
@@ -10616,18 +10679,18 @@
       </c>
     </row>
     <row r="23" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="A23" s="1" t="s">
-        <v>2</v>
+      <c r="A23" t="s">
+        <v>16</v>
       </c>
       <c r="B23">
-        <f t="shared" si="0"/>
+        <f>SUM(C23:W23)</f>
         <v>0</v>
       </c>
       <c r="C23">
         <v>0</v>
       </c>
-      <c r="X23">
-        <v>1</v>
+      <c r="D23">
+        <v>0</v>
       </c>
       <c r="AD23">
         <v>9</v>
@@ -11919,87 +11982,87 @@
       </c>
       <c r="B2">
         <f>Fahrerwertung!C4</f>
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="C2">
         <f>SUM(Fahrerwertung!C4:D4)</f>
-        <v>25</v>
+        <v>38</v>
       </c>
       <c r="D2">
         <f>SUM(Fahrerwertung!C4:E4)</f>
-        <v>25</v>
+        <v>38</v>
       </c>
       <c r="E2">
         <f>SUM(Fahrerwertung!C4:F4)</f>
-        <v>25</v>
+        <v>38</v>
       </c>
       <c r="F2">
         <f>SUM(Fahrerwertung!C4:G4)</f>
-        <v>25</v>
+        <v>38</v>
       </c>
       <c r="G2">
         <f>SUM(Fahrerwertung!C4:H4)</f>
-        <v>25</v>
+        <v>38</v>
       </c>
       <c r="H2">
         <f>SUM(Fahrerwertung!C4:I4)</f>
-        <v>25</v>
+        <v>38</v>
       </c>
       <c r="I2">
         <f>SUM(Fahrerwertung!C4:J4)</f>
-        <v>25</v>
+        <v>38</v>
       </c>
       <c r="J2">
         <f>SUM(Fahrerwertung!C4:K4)</f>
-        <v>25</v>
+        <v>38</v>
       </c>
       <c r="K2">
         <f>SUM(Fahrerwertung!C4:L4)</f>
-        <v>25</v>
+        <v>38</v>
       </c>
       <c r="L2">
         <f>SUM(Fahrerwertung!C4:M4)</f>
-        <v>25</v>
+        <v>38</v>
       </c>
       <c r="M2">
         <f>SUM(Fahrerwertung!C4:N4)</f>
-        <v>25</v>
+        <v>38</v>
       </c>
       <c r="N2">
         <f>SUM(Fahrerwertung!C4:O4)</f>
-        <v>25</v>
+        <v>38</v>
       </c>
       <c r="O2">
         <f>SUM(Fahrerwertung!C4:P4)</f>
-        <v>25</v>
+        <v>38</v>
       </c>
       <c r="P2">
         <f>SUM(Fahrerwertung!C4:Q4)</f>
-        <v>25</v>
+        <v>38</v>
       </c>
       <c r="Q2">
         <f>SUM(Fahrerwertung!C4:R4)</f>
-        <v>25</v>
+        <v>38</v>
       </c>
       <c r="R2">
         <f>SUM(Fahrerwertung!C4:S4)</f>
-        <v>25</v>
+        <v>38</v>
       </c>
       <c r="S2">
         <f>SUM(Fahrerwertung!C4:T4)</f>
-        <v>25</v>
+        <v>38</v>
       </c>
       <c r="T2">
         <f>SUM(Fahrerwertung!C4:U4)</f>
-        <v>25</v>
+        <v>38</v>
       </c>
       <c r="U2">
         <f>SUM(Fahrerwertung!C4:V4)</f>
-        <v>25</v>
+        <v>38</v>
       </c>
       <c r="V2">
         <f>SUM(Fahrerwertung!C4:W4)</f>
-        <v>25</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.2">
@@ -12012,83 +12075,83 @@
       </c>
       <c r="C3">
         <f>SUM(Fahrerwertung!C5:D5)</f>
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="D3">
         <f>SUM(Fahrerwertung!C5:E5)</f>
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="E3">
         <f>SUM(Fahrerwertung!C5:F5)</f>
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="F3">
         <f>SUM(Fahrerwertung!C5:G5)</f>
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="G3">
         <f>SUM(Fahrerwertung!C5:H5)</f>
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="H3">
         <f>SUM(Fahrerwertung!C5:I5)</f>
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="I3">
         <f>SUM(Fahrerwertung!C5:J5)</f>
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="J3">
         <f>SUM(Fahrerwertung!C5:K5)</f>
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="K3">
         <f>SUM(Fahrerwertung!C5:L5)</f>
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="L3">
         <f>SUM(Fahrerwertung!C5:M5)</f>
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="M3">
         <f>SUM(Fahrerwertung!C5:N5)</f>
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="N3">
         <f>SUM(Fahrerwertung!C5:O5)</f>
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="O3">
         <f>SUM(Fahrerwertung!C5:P5)</f>
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="P3">
         <f>SUM(Fahrerwertung!C5:Q5)</f>
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="Q3">
         <f>SUM(Fahrerwertung!C5:R5)</f>
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="R3">
         <f>SUM(Fahrerwertung!C5:S5)</f>
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="S3">
         <f>SUM(Fahrerwertung!C5:T5)</f>
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="T3">
         <f>SUM(Fahrerwertung!C5:U5)</f>
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="U3">
         <f>SUM(Fahrerwertung!C5:V5)</f>
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="V3">
         <f>SUM(Fahrerwertung!C5:W5)</f>
-        <v>18</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.2">
@@ -12097,87 +12160,87 @@
       </c>
       <c r="B4">
         <f>Fahrerwertung!C6</f>
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="C4">
         <f>SUM(Fahrerwertung!C6:D6)</f>
-        <v>15</v>
+        <v>33</v>
       </c>
       <c r="D4">
         <f>SUM(Fahrerwertung!C6:E6)</f>
-        <v>15</v>
+        <v>33</v>
       </c>
       <c r="E4">
         <f>SUM(Fahrerwertung!C6:F6)</f>
-        <v>15</v>
+        <v>33</v>
       </c>
       <c r="F4">
         <f>SUM(Fahrerwertung!C6:G6)</f>
-        <v>15</v>
+        <v>33</v>
       </c>
       <c r="G4">
         <f>SUM(Fahrerwertung!C6:H6)</f>
-        <v>15</v>
+        <v>33</v>
       </c>
       <c r="H4">
         <f>SUM(Fahrerwertung!C6:I6)</f>
-        <v>15</v>
+        <v>33</v>
       </c>
       <c r="I4">
         <f>SUM(Fahrerwertung!C6:J6)</f>
-        <v>15</v>
+        <v>33</v>
       </c>
       <c r="J4">
         <f>SUM(Fahrerwertung!C6:K6)</f>
-        <v>15</v>
+        <v>33</v>
       </c>
       <c r="K4">
         <f>SUM(Fahrerwertung!C6:L6)</f>
-        <v>15</v>
+        <v>33</v>
       </c>
       <c r="L4">
         <f>SUM(Fahrerwertung!C6:M6)</f>
-        <v>15</v>
+        <v>33</v>
       </c>
       <c r="M4">
         <f>SUM(Fahrerwertung!C6:N6)</f>
-        <v>15</v>
+        <v>33</v>
       </c>
       <c r="N4">
         <f>SUM(Fahrerwertung!C6:O6)</f>
-        <v>15</v>
+        <v>33</v>
       </c>
       <c r="O4">
         <f>SUM(Fahrerwertung!C6:P6)</f>
-        <v>15</v>
+        <v>33</v>
       </c>
       <c r="P4">
         <f>SUM(Fahrerwertung!C6:Q6)</f>
-        <v>15</v>
+        <v>33</v>
       </c>
       <c r="Q4">
         <f>SUM(Fahrerwertung!C6:R6)</f>
-        <v>15</v>
+        <v>33</v>
       </c>
       <c r="R4">
         <f>SUM(Fahrerwertung!C6:S6)</f>
-        <v>15</v>
+        <v>33</v>
       </c>
       <c r="S4">
         <f>SUM(Fahrerwertung!C6:T6)</f>
-        <v>15</v>
+        <v>33</v>
       </c>
       <c r="T4">
         <f>SUM(Fahrerwertung!C6:U6)</f>
-        <v>15</v>
+        <v>33</v>
       </c>
       <c r="U4">
         <f>SUM(Fahrerwertung!C6:V6)</f>
-        <v>15</v>
+        <v>33</v>
       </c>
       <c r="V4">
         <f>SUM(Fahrerwertung!C6:W6)</f>
-        <v>15</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.2">
@@ -12186,87 +12249,87 @@
       </c>
       <c r="B5">
         <f>Fahrerwertung!C7</f>
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C5">
         <f>SUM(Fahrerwertung!C7:D7)</f>
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="D5">
         <f>SUM(Fahrerwertung!C7:E7)</f>
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="E5">
         <f>SUM(Fahrerwertung!C7:F7)</f>
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="F5">
         <f>SUM(Fahrerwertung!C7:G7)</f>
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="G5">
         <f>SUM(Fahrerwertung!C7:H7)</f>
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="H5">
         <f>SUM(Fahrerwertung!C7:I7)</f>
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="I5">
         <f>SUM(Fahrerwertung!C7:J7)</f>
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="J5">
         <f>SUM(Fahrerwertung!C7:K7)</f>
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="K5">
         <f>SUM(Fahrerwertung!C7:L7)</f>
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="L5">
         <f>SUM(Fahrerwertung!C7:M7)</f>
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="M5">
         <f>SUM(Fahrerwertung!C7:N7)</f>
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="N5">
         <f>SUM(Fahrerwertung!C7:O7)</f>
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="O5">
         <f>SUM(Fahrerwertung!C7:P7)</f>
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="P5">
         <f>SUM(Fahrerwertung!C7:Q7)</f>
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="Q5">
         <f>SUM(Fahrerwertung!C7:R7)</f>
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="R5">
         <f>SUM(Fahrerwertung!C7:S7)</f>
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="S5">
         <f>SUM(Fahrerwertung!C7:T7)</f>
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="T5">
         <f>SUM(Fahrerwertung!C7:U7)</f>
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="U5">
         <f>SUM(Fahrerwertung!C7:V7)</f>
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="V5">
         <f>SUM(Fahrerwertung!C7:W7)</f>
-        <v>12</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.2">
@@ -12275,87 +12338,87 @@
       </c>
       <c r="B6">
         <f>Fahrerwertung!C8</f>
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C6">
         <f>SUM(Fahrerwertung!C8:D8)</f>
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="D6">
         <f>SUM(Fahrerwertung!C8:E8)</f>
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="E6">
         <f>SUM(Fahrerwertung!C8:F8)</f>
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="F6">
         <f>SUM(Fahrerwertung!C8:G8)</f>
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="G6">
         <f>SUM(Fahrerwertung!C8:H8)</f>
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="H6">
         <f>SUM(Fahrerwertung!C8:I8)</f>
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="I6">
         <f>SUM(Fahrerwertung!C8:J8)</f>
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="J6">
         <f>SUM(Fahrerwertung!C8:K8)</f>
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="K6">
         <f>SUM(Fahrerwertung!C8:L8)</f>
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="L6">
         <f>SUM(Fahrerwertung!C8:M8)</f>
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="M6">
         <f>SUM(Fahrerwertung!C8:N8)</f>
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="N6">
         <f>SUM(Fahrerwertung!C8:O8)</f>
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="O6">
         <f>SUM(Fahrerwertung!C8:P8)</f>
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="P6">
         <f>SUM(Fahrerwertung!C8:Q8)</f>
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="Q6">
         <f>SUM(Fahrerwertung!C8:R8)</f>
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="R6">
         <f>SUM(Fahrerwertung!C8:S8)</f>
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="S6">
         <f>SUM(Fahrerwertung!C8:T8)</f>
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="T6">
         <f>SUM(Fahrerwertung!C8:U8)</f>
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="U6">
         <f>SUM(Fahrerwertung!C8:V8)</f>
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="V6">
         <f>SUM(Fahrerwertung!C8:W8)</f>
-        <v>10</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.2">
@@ -12364,87 +12427,87 @@
       </c>
       <c r="B7">
         <f>Fahrerwertung!C9</f>
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="C7">
         <f>SUM(Fahrerwertung!C9:D9)</f>
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="D7">
         <f>SUM(Fahrerwertung!C9:E9)</f>
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="E7">
         <f>SUM(Fahrerwertung!C9:F9)</f>
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="F7">
         <f>SUM(Fahrerwertung!C9:G9)</f>
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="G7">
         <f>SUM(Fahrerwertung!C9:H9)</f>
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="H7">
         <f>SUM(Fahrerwertung!C9:I9)</f>
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="I7">
         <f>SUM(Fahrerwertung!C9:J9)</f>
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="J7">
         <f>SUM(Fahrerwertung!C9:K9)</f>
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="K7">
         <f>SUM(Fahrerwertung!C9:L9)</f>
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="L7">
         <f>SUM(Fahrerwertung!C9:M9)</f>
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="M7">
         <f>SUM(Fahrerwertung!C9:N9)</f>
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="N7">
         <f>SUM(Fahrerwertung!C9:O9)</f>
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="O7">
         <f>SUM(Fahrerwertung!C9:P9)</f>
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="P7">
         <f>SUM(Fahrerwertung!C9:Q9)</f>
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="Q7">
         <f>SUM(Fahrerwertung!C9:R9)</f>
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="R7">
         <f>SUM(Fahrerwertung!C9:S9)</f>
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="S7">
         <f>SUM(Fahrerwertung!C9:T9)</f>
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="T7">
         <f>SUM(Fahrerwertung!C9:U9)</f>
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="U7">
         <f>SUM(Fahrerwertung!C9:V9)</f>
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="V7">
         <f>SUM(Fahrerwertung!C9:W9)</f>
-        <v>8</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.2">
@@ -12453,87 +12516,87 @@
       </c>
       <c r="B8">
         <f>Fahrerwertung!C10</f>
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C8">
         <f>SUM(Fahrerwertung!C10:D10)</f>
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="D8">
         <f>SUM(Fahrerwertung!C10:E10)</f>
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="E8">
         <f>SUM(Fahrerwertung!C10:F10)</f>
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="F8">
         <f>SUM(Fahrerwertung!C10:G10)</f>
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="G8">
         <f>SUM(Fahrerwertung!C10:H10)</f>
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="H8">
         <f>SUM(Fahrerwertung!C10:I10)</f>
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="I8">
         <f>SUM(Fahrerwertung!C10:J10)</f>
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="J8">
         <f>SUM(Fahrerwertung!C10:K10)</f>
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="K8">
         <f>SUM(Fahrerwertung!C10:L10)</f>
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="L8">
         <f>SUM(Fahrerwertung!C10:M10)</f>
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="M8">
         <f>SUM(Fahrerwertung!C10:N10)</f>
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="N8">
         <f>SUM(Fahrerwertung!C10:O10)</f>
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="O8">
         <f>SUM(Fahrerwertung!C10:P10)</f>
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="P8">
         <f>SUM(Fahrerwertung!C10:Q10)</f>
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="Q8">
         <f>SUM(Fahrerwertung!C10:R10)</f>
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="R8">
         <f>SUM(Fahrerwertung!C10:S10)</f>
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="S8">
         <f>SUM(Fahrerwertung!C10:T10)</f>
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="T8">
         <f>SUM(Fahrerwertung!C10:U10)</f>
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="U8">
         <f>SUM(Fahrerwertung!C10:V10)</f>
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="V8">
         <f>SUM(Fahrerwertung!C10:W10)</f>
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.2">
@@ -12542,87 +12605,87 @@
       </c>
       <c r="B9">
         <f>Fahrerwertung!C11</f>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C9">
         <f>SUM(Fahrerwertung!C11:D11)</f>
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="D9">
         <f>SUM(Fahrerwertung!C11:E11)</f>
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="E9">
         <f>SUM(Fahrerwertung!C11:F11)</f>
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="F9">
         <f>SUM(Fahrerwertung!C11:G11)</f>
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="G9">
         <f>SUM(Fahrerwertung!C11:H11)</f>
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="H9">
         <f>SUM(Fahrerwertung!C11:I11)</f>
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="I9">
         <f>SUM(Fahrerwertung!C11:J11)</f>
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="J9">
         <f>SUM(Fahrerwertung!C11:K11)</f>
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="K9">
         <f>SUM(Fahrerwertung!C11:L11)</f>
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="L9">
         <f>SUM(Fahrerwertung!C11:M11)</f>
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="M9">
         <f>SUM(Fahrerwertung!C11:N11)</f>
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="N9">
         <f>SUM(Fahrerwertung!C11:O11)</f>
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="O9">
         <f>SUM(Fahrerwertung!C11:P11)</f>
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="P9">
         <f>SUM(Fahrerwertung!C11:Q11)</f>
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="Q9">
         <f>SUM(Fahrerwertung!C11:R11)</f>
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="R9">
         <f>SUM(Fahrerwertung!C11:S11)</f>
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="S9">
         <f>SUM(Fahrerwertung!C11:T11)</f>
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="T9">
         <f>SUM(Fahrerwertung!C11:U11)</f>
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="U9">
         <f>SUM(Fahrerwertung!C11:V11)</f>
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="V9">
         <f>SUM(Fahrerwertung!C11:W11)</f>
-        <v>4</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.2">
@@ -12631,87 +12694,87 @@
       </c>
       <c r="B10">
         <f>Fahrerwertung!C12</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C10">
         <f>SUM(Fahrerwertung!C12:D12)</f>
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="D10">
         <f>SUM(Fahrerwertung!C12:E12)</f>
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="E10">
         <f>SUM(Fahrerwertung!C12:F12)</f>
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="F10">
         <f>SUM(Fahrerwertung!C12:G12)</f>
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="G10">
         <f>SUM(Fahrerwertung!C12:H12)</f>
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="H10">
         <f>SUM(Fahrerwertung!C12:I12)</f>
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="I10">
         <f>SUM(Fahrerwertung!C12:J12)</f>
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="J10">
         <f>SUM(Fahrerwertung!C12:K12)</f>
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="K10">
         <f>SUM(Fahrerwertung!C12:L12)</f>
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="L10">
         <f>SUM(Fahrerwertung!C12:M12)</f>
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="M10">
         <f>SUM(Fahrerwertung!C12:N12)</f>
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="N10">
         <f>SUM(Fahrerwertung!C12:O12)</f>
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="O10">
         <f>SUM(Fahrerwertung!C12:P12)</f>
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="P10">
         <f>SUM(Fahrerwertung!C12:Q12)</f>
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="Q10">
         <f>SUM(Fahrerwertung!C12:R12)</f>
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="R10">
         <f>SUM(Fahrerwertung!C12:S12)</f>
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="S10">
         <f>SUM(Fahrerwertung!C12:T12)</f>
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="T10">
         <f>SUM(Fahrerwertung!C12:U12)</f>
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="U10">
         <f>SUM(Fahrerwertung!C12:V12)</f>
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="V10">
         <f>SUM(Fahrerwertung!C12:W12)</f>
-        <v>3</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.2">
@@ -12720,87 +12783,87 @@
       </c>
       <c r="B11">
         <f>Fahrerwertung!C13</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C11">
         <f>SUM(Fahrerwertung!C13:D13)</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D11">
         <f>SUM(Fahrerwertung!C13:E13)</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E11">
         <f>SUM(Fahrerwertung!C13:F13)</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F11">
         <f>SUM(Fahrerwertung!C13:G13)</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G11">
         <f>SUM(Fahrerwertung!C13:H13)</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H11">
         <f>SUM(Fahrerwertung!C13:I13)</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I11">
         <f>SUM(Fahrerwertung!C13:J13)</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="J11">
         <f>SUM(Fahrerwertung!C13:K13)</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="K11">
         <f>SUM(Fahrerwertung!C13:L13)</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="L11">
         <f>SUM(Fahrerwertung!C13:M13)</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="M11">
         <f>SUM(Fahrerwertung!C13:N13)</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="N11">
         <f>SUM(Fahrerwertung!C13:O13)</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="O11">
         <f>SUM(Fahrerwertung!C13:P13)</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="P11">
         <f>SUM(Fahrerwertung!C13:Q13)</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="Q11">
         <f>SUM(Fahrerwertung!C13:R13)</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="R11">
         <f>SUM(Fahrerwertung!C13:S13)</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="S11">
         <f>SUM(Fahrerwertung!C13:T13)</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="T11">
         <f>SUM(Fahrerwertung!C13:U13)</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="U11">
         <f>SUM(Fahrerwertung!C13:V13)</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="V11">
         <f>SUM(Fahrerwertung!C13:W13)</f>
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.2">
@@ -12809,87 +12872,87 @@
       </c>
       <c r="B12">
         <f>Fahrerwertung!C14</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C12">
         <f>SUM(Fahrerwertung!C14:D14)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D12">
         <f>SUM(Fahrerwertung!C14:E14)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E12">
         <f>SUM(Fahrerwertung!C14:F14)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F12">
         <f>SUM(Fahrerwertung!C14:G14)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G12">
         <f>SUM(Fahrerwertung!C14:H14)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H12">
         <f>SUM(Fahrerwertung!C14:I14)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I12">
         <f>SUM(Fahrerwertung!C14:J14)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J12">
         <f>SUM(Fahrerwertung!C14:K14)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K12">
         <f>SUM(Fahrerwertung!C14:L14)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L12">
         <f>SUM(Fahrerwertung!C14:M14)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M12">
         <f>SUM(Fahrerwertung!C14:N14)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N12">
         <f>SUM(Fahrerwertung!C14:O14)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O12">
         <f>SUM(Fahrerwertung!C14:P14)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P12">
         <f>SUM(Fahrerwertung!C14:Q14)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q12">
         <f>SUM(Fahrerwertung!C14:R14)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R12">
         <f>SUM(Fahrerwertung!C14:S14)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S12">
         <f>SUM(Fahrerwertung!C14:T14)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T12">
         <f>SUM(Fahrerwertung!C14:U14)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U12">
         <f>SUM(Fahrerwertung!C14:V14)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V12">
         <f>SUM(Fahrerwertung!C14:W14)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.2">
@@ -12902,83 +12965,83 @@
       </c>
       <c r="C13">
         <f>SUM(Fahrerwertung!C15:D15)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D13">
         <f>SUM(Fahrerwertung!C15:E15)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E13">
         <f>SUM(Fahrerwertung!C15:F15)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F13">
         <f>SUM(Fahrerwertung!C15:G15)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G13">
         <f>SUM(Fahrerwertung!C15:H15)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H13">
         <f>SUM(Fahrerwertung!C15:I15)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I13">
         <f>SUM(Fahrerwertung!C15:J15)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J13">
         <f>SUM(Fahrerwertung!C15:K15)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K13">
         <f>SUM(Fahrerwertung!C15:L15)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L13">
         <f>SUM(Fahrerwertung!C15:M15)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M13">
         <f>SUM(Fahrerwertung!C15:N15)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N13">
         <f>SUM(Fahrerwertung!C15:O15)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O13">
         <f>SUM(Fahrerwertung!C15:P15)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P13">
         <f>SUM(Fahrerwertung!C15:Q15)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q13">
         <f>SUM(Fahrerwertung!C15:R15)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R13">
         <f>SUM(Fahrerwertung!C15:S15)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S13">
         <f>SUM(Fahrerwertung!C15:T15)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T13">
         <f>SUM(Fahrerwertung!C15:U15)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U13">
         <f>SUM(Fahrerwertung!C15:V15)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V13">
         <f>SUM(Fahrerwertung!C15:W15)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
format data for better import
</commit_message>
<xml_diff>
--- a/seasons_excel/Formel1_2019_WM_3.xlsx
+++ b/seasons_excel/Formel1_2019_WM_3.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/timkeller/git_repos/TK5/F1-virtualWC/seasons_excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AE39E71-9A29-C345-BB82-41C1BD7DD4C2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{359AC816-501E-2A4E-9A7E-1BD05AB1239C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="29140" yWindow="-940" windowWidth="35460" windowHeight="20160" xr2:uid="{15EF9A06-B4D9-F442-81AB-3E6205016DF9}"/>
   </bookViews>
@@ -232,7 +232,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -492,16 +492,16 @@
               <c:strCache>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
+                  <c:v>Andi </c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Leclerc</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Hamilton</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>Paul </c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Andi </c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Leclerc</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Hamilton</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>Vettel</c:v>
@@ -510,28 +510,28 @@
                   <c:v>Verstappen</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>Perez</c:v>
+                  <c:v>Lorenz </c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>Sainz</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>Lorenz </c:v>
+                  <c:v>Perez</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>Albon </c:v>
                 </c:pt>
                 <c:pt idx="10">
+                  <c:v>Grosjean</c:v>
+                </c:pt>
+                <c:pt idx="11">
                   <c:v>Räikkönen</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="12">
                   <c:v>Tim </c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="13">
                   <c:v>Gasly</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>Grosjean</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>Hülkenberg</c:v>
@@ -561,46 +561,46 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
+                  <c:v>62</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>38</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>36</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>33</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>23</c:v>
-                </c:pt>
                 <c:pt idx="4">
-                  <c:v>21</c:v>
+                  <c:v>31</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>15</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="6">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>12</c:v>
                 </c:pt>
-                <c:pt idx="7">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>10</c:v>
-                </c:pt>
                 <c:pt idx="9">
-                  <c:v>4</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>0</c:v>
@@ -1001,7 +1001,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Paul </c:v>
+                  <c:v>Andi </c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1037,9 +1037,12 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>12</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>26</c:v>
                 </c:pt>
               </c:numCache>
@@ -1061,7 +1064,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Andi </c:v>
+                  <c:v>Leclerc</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1097,10 +1100,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>18</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>18</c:v>
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1121,7 +1127,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Hamilton</c:v>
+                  <c:v>Paul </c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1157,10 +1163,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>8</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>15</c:v>
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1181,7 +1190,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Perez</c:v>
+                  <c:v>Lorenz </c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1223,10 +1232,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>10</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>2</c:v>
+                <c:pt idx="2">
+                  <c:v>12</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1292,6 +1304,9 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -1660,7 +1675,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Paul </c:v>
+                  <c:v>Andi </c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1682,9 +1697,12 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>12</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>26</c:v>
                 </c:pt>
               </c:numCache>
@@ -1705,7 +1723,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Andi </c:v>
+                  <c:v>Leclerc</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1727,10 +1745,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>18</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>18</c:v>
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2108,10 +2129,10 @@
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>Paul </c:v>
+                  <c:v>Andi </c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Andi </c:v>
+                  <c:v>Leclerc</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2123,10 +2144,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>38</c:v>
+                  <c:v>62</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>36</c:v>
+                  <c:v>41</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2305,10 +2326,10 @@
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>Paul </c:v>
+                  <c:v>Andi </c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Andi </c:v>
+                  <c:v>Leclerc</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2320,10 +2341,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>38</c:v>
+                  <c:v>62</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>36</c:v>
+                  <c:v>41</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2685,67 +2706,67 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>12</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>38</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>38</c:v>
+                  <c:v>62</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>38</c:v>
+                  <c:v>62</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>38</c:v>
+                  <c:v>62</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>38</c:v>
+                  <c:v>62</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>38</c:v>
+                  <c:v>62</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>38</c:v>
+                  <c:v>62</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>38</c:v>
+                  <c:v>62</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>38</c:v>
+                  <c:v>62</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>38</c:v>
+                  <c:v>62</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>38</c:v>
+                  <c:v>62</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>38</c:v>
+                  <c:v>62</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>38</c:v>
+                  <c:v>62</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>38</c:v>
+                  <c:v>62</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>38</c:v>
+                  <c:v>62</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>38</c:v>
+                  <c:v>62</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>38</c:v>
+                  <c:v>62</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>38</c:v>
+                  <c:v>62</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>38</c:v>
+                  <c:v>62</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>38</c:v>
+                  <c:v>62</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2861,67 +2882,67 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>18</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>36</c:v>
+                  <c:v>33</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>36</c:v>
+                  <c:v>41</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>36</c:v>
+                  <c:v>41</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>36</c:v>
+                  <c:v>41</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>36</c:v>
+                  <c:v>41</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>36</c:v>
+                  <c:v>41</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>36</c:v>
+                  <c:v>41</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>36</c:v>
+                  <c:v>41</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>36</c:v>
+                  <c:v>41</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>36</c:v>
+                  <c:v>41</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>36</c:v>
+                  <c:v>41</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>36</c:v>
+                  <c:v>41</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>36</c:v>
+                  <c:v>41</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>36</c:v>
+                  <c:v>41</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>36</c:v>
+                  <c:v>41</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>36</c:v>
+                  <c:v>41</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>36</c:v>
+                  <c:v>41</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>36</c:v>
+                  <c:v>41</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>36</c:v>
+                  <c:v>41</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>36</c:v>
+                  <c:v>41</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3037,67 +3058,67 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>25</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>33</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>33</c:v>
+                  <c:v>41</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>33</c:v>
+                  <c:v>41</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>33</c:v>
+                  <c:v>41</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>33</c:v>
+                  <c:v>41</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>33</c:v>
+                  <c:v>41</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>33</c:v>
+                  <c:v>41</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>33</c:v>
+                  <c:v>41</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>33</c:v>
+                  <c:v>41</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>33</c:v>
+                  <c:v>41</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>33</c:v>
+                  <c:v>41</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>33</c:v>
+                  <c:v>41</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>33</c:v>
+                  <c:v>41</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>33</c:v>
+                  <c:v>41</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>33</c:v>
+                  <c:v>41</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>33</c:v>
+                  <c:v>41</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>33</c:v>
+                  <c:v>41</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>33</c:v>
+                  <c:v>41</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>33</c:v>
+                  <c:v>41</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>33</c:v>
+                  <c:v>41</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3213,67 +3234,67 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>8</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>23</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>23</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>23</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>23</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>23</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>23</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>23</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>23</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>23</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>23</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>23</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>23</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>23</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>23</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>23</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>23</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>23</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>23</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>23</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>23</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3395,61 +3416,61 @@
                   <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>21</c:v>
+                  <c:v>31</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>21</c:v>
+                  <c:v>31</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>21</c:v>
+                  <c:v>31</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>21</c:v>
+                  <c:v>31</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>21</c:v>
+                  <c:v>31</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>21</c:v>
+                  <c:v>31</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>21</c:v>
+                  <c:v>31</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>21</c:v>
+                  <c:v>31</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>21</c:v>
+                  <c:v>31</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>21</c:v>
+                  <c:v>31</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>21</c:v>
+                  <c:v>31</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>21</c:v>
+                  <c:v>31</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>21</c:v>
+                  <c:v>31</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>21</c:v>
+                  <c:v>31</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>21</c:v>
+                  <c:v>31</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>21</c:v>
+                  <c:v>31</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>21</c:v>
+                  <c:v>31</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>21</c:v>
+                  <c:v>31</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>21</c:v>
+                  <c:v>31</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3571,61 +3592,61 @@
                   <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>15</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>15</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>15</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>15</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>15</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>15</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>15</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>15</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>15</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>15</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>15</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>15</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>15</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>15</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>15</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>15</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>15</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>15</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>15</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3743,67 +3764,67 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>10</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>12</c:v>
-                </c:pt>
                 <c:pt idx="2">
-                  <c:v>12</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>12</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>12</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>12</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>12</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>12</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>12</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>12</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>12</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>12</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>12</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>12</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>12</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>12</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>12</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>12</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>12</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>12</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>12</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3927,61 +3948,61 @@
                   <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>10</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>10</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>10</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>10</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>10</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>10</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>10</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>10</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>10</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>10</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>10</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>10</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>10</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>10</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>10</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>10</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>10</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>10</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4099,67 +4120,67 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>10</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>10</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>10</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>10</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>10</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>10</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>10</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>10</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>10</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>10</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>10</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>10</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>10</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>10</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>10</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>10</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>10</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>10</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4283,61 +4304,61 @@
                   <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>4</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>4</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>4</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>4</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>4</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>4</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>4</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>4</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>4</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>4</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>4</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>4</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>4</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4455,67 +4476,67 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4633,7 +4654,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>1</c:v>
@@ -4815,64 +4836,64 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4997,61 +5018,61 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -10178,17 +10199,17 @@
   <dimension ref="A1:AF26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="21.6640625" customWidth="1"/>
     <col min="2" max="2" width="16" customWidth="1"/>
     <col min="6" max="6" width="13.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:32">
       <c r="A1" s="22" t="s">
         <v>50</v>
       </c>
@@ -10196,13 +10217,13 @@
       <c r="C1" s="22"/>
       <c r="D1" s="22"/>
     </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:32">
       <c r="A2" s="22"/>
       <c r="B2" s="22"/>
       <c r="C2" s="22"/>
       <c r="D2" s="22"/>
     </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:32">
       <c r="A3" t="s">
         <v>58</v>
       </c>
@@ -10273,64 +10294,76 @@
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="A4" s="9" t="s">
-        <v>19</v>
+    <row r="4" spans="1:32">
+      <c r="A4" s="3" t="s">
+        <v>4</v>
       </c>
       <c r="B4">
         <f>SUM(C4:W4)</f>
-        <v>38</v>
+        <v>62</v>
       </c>
       <c r="C4">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="D4">
+        <v>18</v>
+      </c>
+      <c r="E4">
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
-        <v>4</v>
+    <row r="5" spans="1:32">
+      <c r="A5" s="2" t="s">
+        <v>6</v>
       </c>
       <c r="B5">
         <f>SUM(C5:W5)</f>
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="C5">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="D5">
-        <v>18</v>
+        <v>8</v>
+      </c>
+      <c r="E5">
+        <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
-        <v>6</v>
+    <row r="6" spans="1:32">
+      <c r="A6" s="1" t="s">
+        <v>61</v>
       </c>
       <c r="B6">
         <f>SUM(C6:W6)</f>
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="C6">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="D6">
-        <v>8</v>
+        <v>15</v>
+      </c>
+      <c r="E6">
+        <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
-        <v>61</v>
+    <row r="7" spans="1:32">
+      <c r="A7" s="9" t="s">
+        <v>19</v>
       </c>
       <c r="B7">
         <f>SUM(C7:W7)</f>
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="C7">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D7">
-        <v>15</v>
+        <v>26</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
       </c>
       <c r="AD7">
         <v>1</v>
@@ -10342,13 +10375,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:32">
       <c r="A8" s="2" t="s">
         <v>59</v>
       </c>
       <c r="B8">
         <f>SUM(C8:W8)</f>
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="C8">
         <v>15</v>
@@ -10356,6 +10389,9 @@
       <c r="D8">
         <v>6</v>
       </c>
+      <c r="E8">
+        <v>10</v>
+      </c>
       <c r="AE8" s="1" t="s">
         <v>61</v>
       </c>
@@ -10363,13 +10399,13 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:32">
       <c r="A9" s="6" t="s">
         <v>7</v>
       </c>
       <c r="B9">
         <f>SUM(C9:W9)</f>
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="C9">
         <v>3</v>
@@ -10377,6 +10413,9 @@
       <c r="D9">
         <v>12</v>
       </c>
+      <c r="E9">
+        <v>15</v>
+      </c>
       <c r="AD9">
         <v>2</v>
       </c>
@@ -10387,19 +10426,22 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="A10" s="9" t="s">
-        <v>12</v>
+    <row r="10" spans="1:32">
+      <c r="A10" s="5" t="s">
+        <v>3</v>
       </c>
       <c r="B10">
         <f>SUM(C10:W10)</f>
+        <v>22</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>10</v>
+      </c>
+      <c r="E10">
         <v>12</v>
-      </c>
-      <c r="C10">
-        <v>10</v>
-      </c>
-      <c r="D10">
-        <v>2</v>
       </c>
       <c r="AE10" s="2" t="s">
         <v>59</v>
@@ -10408,13 +10450,13 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:32">
       <c r="A11" s="3" t="s">
         <v>60</v>
       </c>
       <c r="B11">
         <f>SUM(C11:W11)</f>
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="C11">
         <v>6</v>
@@ -10422,6 +10464,9 @@
       <c r="D11">
         <v>4</v>
       </c>
+      <c r="E11">
+        <v>6</v>
+      </c>
       <c r="AD11">
         <v>3</v>
       </c>
@@ -10432,19 +10477,22 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="A12" s="5" t="s">
-        <v>3</v>
+    <row r="12" spans="1:32">
+      <c r="A12" s="9" t="s">
+        <v>12</v>
       </c>
       <c r="B12">
         <f>SUM(C12:W12)</f>
+        <v>12</v>
+      </c>
+      <c r="C12">
         <v>10</v>
       </c>
-      <c r="C12">
-        <v>0</v>
-      </c>
       <c r="D12">
-        <v>10</v>
+        <v>2</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
       </c>
       <c r="AE12" s="6" t="s">
         <v>15</v>
@@ -10453,13 +10501,13 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:32">
       <c r="A13" s="6" t="s">
         <v>15</v>
       </c>
       <c r="B13">
         <f>SUM(C13:W13)</f>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C13">
         <v>4</v>
@@ -10467,6 +10515,9 @@
       <c r="D13">
         <v>0</v>
       </c>
+      <c r="E13">
+        <v>4</v>
+      </c>
       <c r="AD13">
         <v>4</v>
       </c>
@@ -10477,19 +10528,22 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="A14" s="8" t="s">
-        <v>13</v>
+    <row r="14" spans="1:32">
+      <c r="A14" s="5" t="s">
+        <v>10</v>
       </c>
       <c r="B14">
         <f>SUM(C14:W14)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D14">
         <v>0</v>
+      </c>
+      <c r="E14">
+        <v>2</v>
       </c>
       <c r="AE14" s="5" t="s">
         <v>10</v>
@@ -10498,19 +10552,22 @@
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="A15" s="1" t="s">
-        <v>2</v>
+    <row r="15" spans="1:32">
+      <c r="A15" s="8" t="s">
+        <v>13</v>
       </c>
       <c r="B15">
         <f>SUM(C15:W15)</f>
         <v>1</v>
       </c>
       <c r="C15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D15">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
       </c>
       <c r="AD15">
         <v>5</v>
@@ -10522,18 +10579,21 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="A16" s="7" t="s">
-        <v>8</v>
+    <row r="16" spans="1:32">
+      <c r="A16" s="1" t="s">
+        <v>2</v>
       </c>
       <c r="B16">
         <f>SUM(C16:W16)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C16">
         <v>0</v>
       </c>
       <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16">
         <v>0</v>
       </c>
       <c r="AE16" s="9" t="s">
@@ -10543,19 +10603,22 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="A17" s="5" t="s">
-        <v>10</v>
+    <row r="17" spans="1:32">
+      <c r="A17" s="7" t="s">
+        <v>8</v>
       </c>
       <c r="B17">
         <f>SUM(C17:W17)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C17">
         <v>0</v>
       </c>
       <c r="D17">
         <v>0</v>
+      </c>
+      <c r="E17">
+        <v>1</v>
       </c>
       <c r="AD17">
         <v>6</v>
@@ -10567,7 +10630,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:32">
       <c r="A18" s="4" t="s">
         <v>57</v>
       </c>
@@ -10581,6 +10644,9 @@
       <c r="D18">
         <v>0</v>
       </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
       <c r="AE18" s="3" t="s">
         <v>60</v>
       </c>
@@ -10588,7 +10654,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:32">
       <c r="A19" s="4" t="s">
         <v>9</v>
       </c>
@@ -10602,6 +10668,9 @@
       <c r="D19">
         <v>0</v>
       </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
       <c r="AD19">
         <v>7</v>
       </c>
@@ -10612,7 +10681,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:32">
       <c r="A20" s="8" t="s">
         <v>14</v>
       </c>
@@ -10626,6 +10695,9 @@
       <c r="D20">
         <v>0</v>
       </c>
+      <c r="E20">
+        <v>0</v>
+      </c>
       <c r="AE20" s="4" t="s">
         <v>9</v>
       </c>
@@ -10633,7 +10705,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="21" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:32">
       <c r="A21" t="s">
         <v>17</v>
       </c>
@@ -10647,6 +10719,9 @@
       <c r="D21">
         <v>0</v>
       </c>
+      <c r="E21">
+        <v>0</v>
+      </c>
       <c r="AD21">
         <v>8</v>
       </c>
@@ -10657,7 +10732,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="22" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:32">
       <c r="A22" s="7" t="s">
         <v>18</v>
       </c>
@@ -10671,6 +10746,9 @@
       <c r="D22">
         <v>0</v>
       </c>
+      <c r="E22">
+        <v>0</v>
+      </c>
       <c r="AE22" s="8" t="s">
         <v>14</v>
       </c>
@@ -10678,7 +10756,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="23" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:32">
       <c r="A23" t="s">
         <v>16</v>
       </c>
@@ -10692,6 +10770,9 @@
       <c r="D23">
         <v>0</v>
       </c>
+      <c r="E23">
+        <v>0</v>
+      </c>
       <c r="AD23">
         <v>9</v>
       </c>
@@ -10702,7 +10783,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="24" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:32">
       <c r="AE24" s="7" t="s">
         <v>8</v>
       </c>
@@ -10710,7 +10791,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="25" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:32">
       <c r="AD25">
         <v>10</v>
       </c>
@@ -10721,7 +10802,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="26" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:32">
       <c r="AE26" t="s">
         <v>16</v>
       </c>
@@ -10754,12 +10835,12 @@
       <selection activeCell="W12" sqref="W12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:23" ht="16" customHeight="1">
       <c r="A1" s="23" t="s">
         <v>51</v>
       </c>
@@ -10786,7 +10867,7 @@
       <c r="V1" s="10"/>
       <c r="W1" s="10"/>
     </row>
-    <row r="2" spans="1:23" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:23" ht="16" customHeight="1">
       <c r="A2" s="23"/>
       <c r="B2" s="23"/>
       <c r="C2" s="23"/>
@@ -10811,7 +10892,7 @@
       <c r="V2" s="10"/>
       <c r="W2" s="10"/>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:23">
       <c r="A3" s="10" t="s">
         <v>0</v>
       </c>
@@ -10882,7 +10963,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:23">
       <c r="A4" s="18" t="s">
         <v>55</v>
       </c>
@@ -10965,7 +11046,7 @@
       </c>
       <c r="W4" s="10"/>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:23">
       <c r="A5" s="19" t="s">
         <v>56</v>
       </c>
@@ -11040,7 +11121,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:23">
       <c r="A6" s="14" t="s">
         <v>53</v>
       </c>
@@ -11110,7 +11191,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:23">
       <c r="A7" s="13" t="s">
         <v>52</v>
       </c>
@@ -11182,7 +11263,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:23">
       <c r="A8" s="16" t="s">
         <v>54</v>
       </c>
@@ -11257,7 +11338,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:23">
       <c r="A9" s="21" t="s">
         <v>43</v>
       </c>
@@ -11321,7 +11402,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:23">
       <c r="A10" s="15" t="s">
         <v>44</v>
       </c>
@@ -11380,7 +11461,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:23">
       <c r="A11" s="17" t="s">
         <v>42</v>
       </c>
@@ -11440,7 +11521,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:23">
       <c r="A12" s="20" t="s">
         <v>45</v>
       </c>
@@ -11478,7 +11559,7 @@
       <c r="V12" s="10"/>
       <c r="W12" s="10"/>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:23">
       <c r="A13" s="11" t="s">
         <v>46</v>
       </c>
@@ -11512,7 +11593,7 @@
       <c r="V13" s="10"/>
       <c r="W13" s="10"/>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:23">
       <c r="A14" s="11"/>
       <c r="B14" s="10"/>
       <c r="C14" s="10"/>
@@ -11537,7 +11618,7 @@
       <c r="V14" s="10"/>
       <c r="W14" s="10"/>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:23">
       <c r="A15" s="11"/>
       <c r="B15" s="10"/>
       <c r="C15" s="10"/>
@@ -11562,7 +11643,7 @@
       <c r="V15" s="10"/>
       <c r="W15" s="10"/>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:23">
       <c r="A16" s="11"/>
       <c r="B16" s="10"/>
       <c r="C16" s="10"/>
@@ -11587,7 +11668,7 @@
       <c r="V16" s="10"/>
       <c r="W16" s="10"/>
     </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:23">
       <c r="A17" s="11"/>
       <c r="B17" s="10"/>
       <c r="C17" s="10"/>
@@ -11612,7 +11693,7 @@
       <c r="V17" s="10"/>
       <c r="W17" s="10"/>
     </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:23">
       <c r="A18" s="11"/>
       <c r="B18" s="10"/>
       <c r="C18" s="10"/>
@@ -11637,7 +11718,7 @@
       <c r="V18" s="10"/>
       <c r="W18" s="10"/>
     </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:23">
       <c r="A19" s="11"/>
       <c r="B19" s="10"/>
       <c r="C19" s="10"/>
@@ -11662,7 +11743,7 @@
       <c r="V19" s="10"/>
       <c r="W19" s="10"/>
     </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:23">
       <c r="A20" s="11"/>
       <c r="B20" s="10"/>
       <c r="C20" s="10"/>
@@ -11687,7 +11768,7 @@
       <c r="V20" s="10"/>
       <c r="W20" s="10"/>
     </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:23">
       <c r="A21" s="11"/>
       <c r="B21" s="10"/>
       <c r="C21" s="10"/>
@@ -11712,7 +11793,7 @@
       <c r="V21" s="10"/>
       <c r="W21" s="10"/>
     </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:23">
       <c r="A22" s="11"/>
       <c r="B22" s="10"/>
       <c r="C22" s="10"/>
@@ -11737,7 +11818,7 @@
       <c r="V22" s="10"/>
       <c r="W22" s="10"/>
     </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:23">
       <c r="A23" s="11"/>
       <c r="B23" s="10"/>
       <c r="C23" s="10"/>
@@ -11762,7 +11843,7 @@
       <c r="V23" s="10"/>
       <c r="W23" s="10"/>
     </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:23">
       <c r="A24" s="12"/>
     </row>
   </sheetData>
@@ -11789,12 +11870,12 @@
       <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="20.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>47</v>
       </c>
@@ -11802,7 +11883,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -11810,7 +11891,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -11818,7 +11899,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -11826,7 +11907,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -11834,7 +11915,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -11842,7 +11923,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -11850,7 +11931,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -11858,7 +11939,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -11866,7 +11947,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -11874,7 +11955,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -11882,7 +11963,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2">
       <c r="A12" t="s">
         <v>49</v>
       </c>
@@ -11903,12 +11984,12 @@
       <selection activeCell="V21" sqref="B2:V21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="5" max="5" width="12.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:22">
       <c r="A1" t="s">
         <v>58</v>
       </c>
@@ -11976,363 +12057,363 @@
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:22">
       <c r="A2" s="3" t="s">
         <v>19</v>
       </c>
       <c r="B2">
         <f>Fahrerwertung!C4</f>
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="C2">
         <f>SUM(Fahrerwertung!C4:D4)</f>
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D2">
         <f>SUM(Fahrerwertung!C4:E4)</f>
-        <v>38</v>
+        <v>62</v>
       </c>
       <c r="E2">
         <f>SUM(Fahrerwertung!C4:F4)</f>
-        <v>38</v>
+        <v>62</v>
       </c>
       <c r="F2">
         <f>SUM(Fahrerwertung!C4:G4)</f>
-        <v>38</v>
+        <v>62</v>
       </c>
       <c r="G2">
         <f>SUM(Fahrerwertung!C4:H4)</f>
-        <v>38</v>
+        <v>62</v>
       </c>
       <c r="H2">
         <f>SUM(Fahrerwertung!C4:I4)</f>
-        <v>38</v>
+        <v>62</v>
       </c>
       <c r="I2">
         <f>SUM(Fahrerwertung!C4:J4)</f>
-        <v>38</v>
+        <v>62</v>
       </c>
       <c r="J2">
         <f>SUM(Fahrerwertung!C4:K4)</f>
-        <v>38</v>
+        <v>62</v>
       </c>
       <c r="K2">
         <f>SUM(Fahrerwertung!C4:L4)</f>
-        <v>38</v>
+        <v>62</v>
       </c>
       <c r="L2">
         <f>SUM(Fahrerwertung!C4:M4)</f>
-        <v>38</v>
+        <v>62</v>
       </c>
       <c r="M2">
         <f>SUM(Fahrerwertung!C4:N4)</f>
-        <v>38</v>
+        <v>62</v>
       </c>
       <c r="N2">
         <f>SUM(Fahrerwertung!C4:O4)</f>
-        <v>38</v>
+        <v>62</v>
       </c>
       <c r="O2">
         <f>SUM(Fahrerwertung!C4:P4)</f>
-        <v>38</v>
+        <v>62</v>
       </c>
       <c r="P2">
         <f>SUM(Fahrerwertung!C4:Q4)</f>
-        <v>38</v>
+        <v>62</v>
       </c>
       <c r="Q2">
         <f>SUM(Fahrerwertung!C4:R4)</f>
-        <v>38</v>
+        <v>62</v>
       </c>
       <c r="R2">
         <f>SUM(Fahrerwertung!C4:S4)</f>
-        <v>38</v>
+        <v>62</v>
       </c>
       <c r="S2">
         <f>SUM(Fahrerwertung!C4:T4)</f>
-        <v>38</v>
+        <v>62</v>
       </c>
       <c r="T2">
         <f>SUM(Fahrerwertung!C4:U4)</f>
-        <v>38</v>
+        <v>62</v>
       </c>
       <c r="U2">
         <f>SUM(Fahrerwertung!C4:V4)</f>
-        <v>38</v>
+        <v>62</v>
       </c>
       <c r="V2">
         <f>SUM(Fahrerwertung!C4:W4)</f>
-        <v>38</v>
+        <v>62</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:22">
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B3">
         <f>Fahrerwertung!C5</f>
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="C3">
         <f>SUM(Fahrerwertung!C5:D5)</f>
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D3">
         <f>SUM(Fahrerwertung!C5:E5)</f>
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="E3">
         <f>SUM(Fahrerwertung!C5:F5)</f>
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="F3">
         <f>SUM(Fahrerwertung!C5:G5)</f>
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="G3">
         <f>SUM(Fahrerwertung!C5:H5)</f>
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="H3">
         <f>SUM(Fahrerwertung!C5:I5)</f>
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="I3">
         <f>SUM(Fahrerwertung!C5:J5)</f>
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="J3">
         <f>SUM(Fahrerwertung!C5:K5)</f>
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="K3">
         <f>SUM(Fahrerwertung!C5:L5)</f>
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="L3">
         <f>SUM(Fahrerwertung!C5:M5)</f>
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="M3">
         <f>SUM(Fahrerwertung!C5:N5)</f>
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="N3">
         <f>SUM(Fahrerwertung!C5:O5)</f>
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="O3">
         <f>SUM(Fahrerwertung!C5:P5)</f>
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="P3">
         <f>SUM(Fahrerwertung!C5:Q5)</f>
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="Q3">
         <f>SUM(Fahrerwertung!C5:R5)</f>
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="R3">
         <f>SUM(Fahrerwertung!C5:S5)</f>
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="S3">
         <f>SUM(Fahrerwertung!C5:T5)</f>
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="T3">
         <f>SUM(Fahrerwertung!C5:U5)</f>
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="U3">
         <f>SUM(Fahrerwertung!C5:V5)</f>
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="V3">
         <f>SUM(Fahrerwertung!C5:W5)</f>
-        <v>36</v>
+        <v>41</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:22">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B4">
         <f>Fahrerwertung!C6</f>
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="C4">
         <f>SUM(Fahrerwertung!C6:D6)</f>
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="D4">
         <f>SUM(Fahrerwertung!C6:E6)</f>
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="E4">
         <f>SUM(Fahrerwertung!C6:F6)</f>
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="F4">
         <f>SUM(Fahrerwertung!C6:G6)</f>
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="G4">
         <f>SUM(Fahrerwertung!C6:H6)</f>
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="H4">
         <f>SUM(Fahrerwertung!C6:I6)</f>
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="I4">
         <f>SUM(Fahrerwertung!C6:J6)</f>
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="J4">
         <f>SUM(Fahrerwertung!C6:K6)</f>
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="K4">
         <f>SUM(Fahrerwertung!C6:L6)</f>
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="L4">
         <f>SUM(Fahrerwertung!C6:M6)</f>
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="M4">
         <f>SUM(Fahrerwertung!C6:N6)</f>
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="N4">
         <f>SUM(Fahrerwertung!C6:O6)</f>
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="O4">
         <f>SUM(Fahrerwertung!C6:P6)</f>
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="P4">
         <f>SUM(Fahrerwertung!C6:Q6)</f>
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="Q4">
         <f>SUM(Fahrerwertung!C6:R6)</f>
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="R4">
         <f>SUM(Fahrerwertung!C6:S6)</f>
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="S4">
         <f>SUM(Fahrerwertung!C6:T6)</f>
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="T4">
         <f>SUM(Fahrerwertung!C6:U6)</f>
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="U4">
         <f>SUM(Fahrerwertung!C6:V6)</f>
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="V4">
         <f>SUM(Fahrerwertung!C6:W6)</f>
-        <v>33</v>
+        <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:22">
       <c r="A5" s="9" t="s">
         <v>3</v>
       </c>
       <c r="B5">
         <f>Fahrerwertung!C7</f>
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C5">
         <f>SUM(Fahrerwertung!C7:D7)</f>
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="D5">
         <f>SUM(Fahrerwertung!C7:E7)</f>
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="E5">
         <f>SUM(Fahrerwertung!C7:F7)</f>
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="F5">
         <f>SUM(Fahrerwertung!C7:G7)</f>
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="G5">
         <f>SUM(Fahrerwertung!C7:H7)</f>
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="H5">
         <f>SUM(Fahrerwertung!C7:I7)</f>
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="I5">
         <f>SUM(Fahrerwertung!C7:J7)</f>
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="J5">
         <f>SUM(Fahrerwertung!C7:K7)</f>
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="K5">
         <f>SUM(Fahrerwertung!C7:L7)</f>
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="L5">
         <f>SUM(Fahrerwertung!C7:M7)</f>
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="M5">
         <f>SUM(Fahrerwertung!C7:N7)</f>
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="N5">
         <f>SUM(Fahrerwertung!C7:O7)</f>
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="O5">
         <f>SUM(Fahrerwertung!C7:P7)</f>
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="P5">
         <f>SUM(Fahrerwertung!C7:Q7)</f>
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="Q5">
         <f>SUM(Fahrerwertung!C7:R7)</f>
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="R5">
         <f>SUM(Fahrerwertung!C7:S7)</f>
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="S5">
         <f>SUM(Fahrerwertung!C7:T7)</f>
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="T5">
         <f>SUM(Fahrerwertung!C7:U7)</f>
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="U5">
         <f>SUM(Fahrerwertung!C7:V7)</f>
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="V5">
         <f>SUM(Fahrerwertung!C7:W7)</f>
-        <v>23</v>
+        <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:22">
       <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
@@ -12346,82 +12427,82 @@
       </c>
       <c r="D6">
         <f>SUM(Fahrerwertung!C8:E8)</f>
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="E6">
         <f>SUM(Fahrerwertung!C8:F8)</f>
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="F6">
         <f>SUM(Fahrerwertung!C8:G8)</f>
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="G6">
         <f>SUM(Fahrerwertung!C8:H8)</f>
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="H6">
         <f>SUM(Fahrerwertung!C8:I8)</f>
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="I6">
         <f>SUM(Fahrerwertung!C8:J8)</f>
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="J6">
         <f>SUM(Fahrerwertung!C8:K8)</f>
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="K6">
         <f>SUM(Fahrerwertung!C8:L8)</f>
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="L6">
         <f>SUM(Fahrerwertung!C8:M8)</f>
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="M6">
         <f>SUM(Fahrerwertung!C8:N8)</f>
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="N6">
         <f>SUM(Fahrerwertung!C8:O8)</f>
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="O6">
         <f>SUM(Fahrerwertung!C8:P8)</f>
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="P6">
         <f>SUM(Fahrerwertung!C8:Q8)</f>
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="Q6">
         <f>SUM(Fahrerwertung!C8:R8)</f>
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="R6">
         <f>SUM(Fahrerwertung!C8:S8)</f>
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="S6">
         <f>SUM(Fahrerwertung!C8:T8)</f>
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="T6">
         <f>SUM(Fahrerwertung!C8:U8)</f>
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="U6">
         <f>SUM(Fahrerwertung!C8:V8)</f>
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="V6">
         <f>SUM(Fahrerwertung!C8:W8)</f>
-        <v>21</v>
+        <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:22">
       <c r="A7" s="6" t="s">
         <v>7</v>
       </c>
@@ -12435,171 +12516,171 @@
       </c>
       <c r="D7">
         <f>SUM(Fahrerwertung!C9:E9)</f>
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="E7">
         <f>SUM(Fahrerwertung!C9:F9)</f>
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="F7">
         <f>SUM(Fahrerwertung!C9:G9)</f>
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="G7">
         <f>SUM(Fahrerwertung!C9:H9)</f>
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="H7">
         <f>SUM(Fahrerwertung!C9:I9)</f>
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="I7">
         <f>SUM(Fahrerwertung!C9:J9)</f>
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="J7">
         <f>SUM(Fahrerwertung!C9:K9)</f>
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="K7">
         <f>SUM(Fahrerwertung!C9:L9)</f>
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="L7">
         <f>SUM(Fahrerwertung!C9:M9)</f>
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="M7">
         <f>SUM(Fahrerwertung!C9:N9)</f>
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="N7">
         <f>SUM(Fahrerwertung!C9:O9)</f>
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="O7">
         <f>SUM(Fahrerwertung!C9:P9)</f>
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="P7">
         <f>SUM(Fahrerwertung!C9:Q9)</f>
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="Q7">
         <f>SUM(Fahrerwertung!C9:R9)</f>
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="R7">
         <f>SUM(Fahrerwertung!C9:S9)</f>
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="S7">
         <f>SUM(Fahrerwertung!C9:T9)</f>
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="T7">
         <f>SUM(Fahrerwertung!C9:U9)</f>
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="U7">
         <f>SUM(Fahrerwertung!C9:V9)</f>
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="V7">
         <f>SUM(Fahrerwertung!C9:W9)</f>
-        <v>15</v>
+        <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:22">
       <c r="A8" s="2" t="s">
         <v>20</v>
       </c>
       <c r="B8">
         <f>Fahrerwertung!C10</f>
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="C8">
         <f>SUM(Fahrerwertung!C10:D10)</f>
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D8">
         <f>SUM(Fahrerwertung!C10:E10)</f>
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="E8">
         <f>SUM(Fahrerwertung!C10:F10)</f>
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="F8">
         <f>SUM(Fahrerwertung!C10:G10)</f>
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="G8">
         <f>SUM(Fahrerwertung!C10:H10)</f>
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="H8">
         <f>SUM(Fahrerwertung!C10:I10)</f>
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="I8">
         <f>SUM(Fahrerwertung!C10:J10)</f>
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="J8">
         <f>SUM(Fahrerwertung!C10:K10)</f>
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="K8">
         <f>SUM(Fahrerwertung!C10:L10)</f>
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="L8">
         <f>SUM(Fahrerwertung!C10:M10)</f>
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="M8">
         <f>SUM(Fahrerwertung!C10:N10)</f>
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="N8">
         <f>SUM(Fahrerwertung!C10:O10)</f>
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="O8">
         <f>SUM(Fahrerwertung!C10:P10)</f>
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="P8">
         <f>SUM(Fahrerwertung!C10:Q10)</f>
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="Q8">
         <f>SUM(Fahrerwertung!C10:R10)</f>
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="R8">
         <f>SUM(Fahrerwertung!C10:S10)</f>
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="S8">
         <f>SUM(Fahrerwertung!C10:T10)</f>
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="T8">
         <f>SUM(Fahrerwertung!C10:U10)</f>
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="U8">
         <f>SUM(Fahrerwertung!C10:V10)</f>
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="V8">
         <f>SUM(Fahrerwertung!C10:W10)</f>
-        <v>12</v>
+        <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:22">
       <c r="A9" s="9" t="s">
         <v>12</v>
       </c>
@@ -12613,171 +12694,171 @@
       </c>
       <c r="D9">
         <f>SUM(Fahrerwertung!C11:E11)</f>
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="E9">
         <f>SUM(Fahrerwertung!C11:F11)</f>
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="F9">
         <f>SUM(Fahrerwertung!C11:G11)</f>
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="G9">
         <f>SUM(Fahrerwertung!C11:H11)</f>
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="H9">
         <f>SUM(Fahrerwertung!C11:I11)</f>
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="I9">
         <f>SUM(Fahrerwertung!C11:J11)</f>
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="J9">
         <f>SUM(Fahrerwertung!C11:K11)</f>
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="K9">
         <f>SUM(Fahrerwertung!C11:L11)</f>
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="L9">
         <f>SUM(Fahrerwertung!C11:M11)</f>
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="M9">
         <f>SUM(Fahrerwertung!C11:N11)</f>
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="N9">
         <f>SUM(Fahrerwertung!C11:O11)</f>
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="O9">
         <f>SUM(Fahrerwertung!C11:P11)</f>
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="P9">
         <f>SUM(Fahrerwertung!C11:Q11)</f>
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="Q9">
         <f>SUM(Fahrerwertung!C11:R11)</f>
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="R9">
         <f>SUM(Fahrerwertung!C11:S11)</f>
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="S9">
         <f>SUM(Fahrerwertung!C11:T11)</f>
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="T9">
         <f>SUM(Fahrerwertung!C11:U11)</f>
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="U9">
         <f>SUM(Fahrerwertung!C11:V11)</f>
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="V9">
         <f>SUM(Fahrerwertung!C11:W11)</f>
-        <v>10</v>
+        <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:22">
       <c r="A10" s="7" t="s">
         <v>8</v>
       </c>
       <c r="B10">
         <f>Fahrerwertung!C12</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C10">
         <f>SUM(Fahrerwertung!C12:D12)</f>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D10">
         <f>SUM(Fahrerwertung!C12:E12)</f>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E10">
         <f>SUM(Fahrerwertung!C12:F12)</f>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F10">
         <f>SUM(Fahrerwertung!C12:G12)</f>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G10">
         <f>SUM(Fahrerwertung!C12:H12)</f>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="H10">
         <f>SUM(Fahrerwertung!C12:I12)</f>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="I10">
         <f>SUM(Fahrerwertung!C12:J12)</f>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="J10">
         <f>SUM(Fahrerwertung!C12:K12)</f>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="K10">
         <f>SUM(Fahrerwertung!C12:L12)</f>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="L10">
         <f>SUM(Fahrerwertung!C12:M12)</f>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="M10">
         <f>SUM(Fahrerwertung!C12:N12)</f>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="N10">
         <f>SUM(Fahrerwertung!C12:O12)</f>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="O10">
         <f>SUM(Fahrerwertung!C12:P12)</f>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="P10">
         <f>SUM(Fahrerwertung!C12:Q12)</f>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="Q10">
         <f>SUM(Fahrerwertung!C12:R12)</f>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="R10">
         <f>SUM(Fahrerwertung!C12:S12)</f>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="S10">
         <f>SUM(Fahrerwertung!C12:T12)</f>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="T10">
         <f>SUM(Fahrerwertung!C12:U12)</f>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="U10">
         <f>SUM(Fahrerwertung!C12:V12)</f>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="V10">
         <f>SUM(Fahrerwertung!C12:W12)</f>
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:22">
       <c r="A11" s="5" t="s">
         <v>10</v>
       </c>
@@ -12791,177 +12872,177 @@
       </c>
       <c r="D11">
         <f>SUM(Fahrerwertung!C13:E13)</f>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="E11">
         <f>SUM(Fahrerwertung!C13:F13)</f>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="F11">
         <f>SUM(Fahrerwertung!C13:G13)</f>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="G11">
         <f>SUM(Fahrerwertung!C13:H13)</f>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="H11">
         <f>SUM(Fahrerwertung!C13:I13)</f>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="I11">
         <f>SUM(Fahrerwertung!C13:J13)</f>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="J11">
         <f>SUM(Fahrerwertung!C13:K13)</f>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="K11">
         <f>SUM(Fahrerwertung!C13:L13)</f>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="L11">
         <f>SUM(Fahrerwertung!C13:M13)</f>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="M11">
         <f>SUM(Fahrerwertung!C13:N13)</f>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="N11">
         <f>SUM(Fahrerwertung!C13:O13)</f>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="O11">
         <f>SUM(Fahrerwertung!C13:P13)</f>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="P11">
         <f>SUM(Fahrerwertung!C13:Q13)</f>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="Q11">
         <f>SUM(Fahrerwertung!C13:R13)</f>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="R11">
         <f>SUM(Fahrerwertung!C13:S13)</f>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="S11">
         <f>SUM(Fahrerwertung!C13:T13)</f>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="T11">
         <f>SUM(Fahrerwertung!C13:U13)</f>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="U11">
         <f>SUM(Fahrerwertung!C13:V13)</f>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="V11">
         <f>SUM(Fahrerwertung!C13:W13)</f>
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:22">
       <c r="A12" s="8" t="s">
         <v>13</v>
       </c>
       <c r="B12">
         <f>Fahrerwertung!C14</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C12">
         <f>SUM(Fahrerwertung!C14:D14)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D12">
         <f>SUM(Fahrerwertung!C14:E14)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E12">
         <f>SUM(Fahrerwertung!C14:F14)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F12">
         <f>SUM(Fahrerwertung!C14:G14)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G12">
         <f>SUM(Fahrerwertung!C14:H14)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H12">
         <f>SUM(Fahrerwertung!C14:I14)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I12">
         <f>SUM(Fahrerwertung!C14:J14)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J12">
         <f>SUM(Fahrerwertung!C14:K14)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K12">
         <f>SUM(Fahrerwertung!C14:L14)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L12">
         <f>SUM(Fahrerwertung!C14:M14)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M12">
         <f>SUM(Fahrerwertung!C14:N14)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N12">
         <f>SUM(Fahrerwertung!C14:O14)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O12">
         <f>SUM(Fahrerwertung!C14:P14)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P12">
         <f>SUM(Fahrerwertung!C14:Q14)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Q12">
         <f>SUM(Fahrerwertung!C14:R14)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R12">
         <f>SUM(Fahrerwertung!C14:S14)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="S12">
         <f>SUM(Fahrerwertung!C14:T14)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="T12">
         <f>SUM(Fahrerwertung!C14:U14)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="U12">
         <f>SUM(Fahrerwertung!C14:V14)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="V12">
         <f>SUM(Fahrerwertung!C14:W14)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:22">
       <c r="A13" s="6" t="s">
         <v>15</v>
       </c>
       <c r="B13">
         <f>Fahrerwertung!C15</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C13">
         <f>SUM(Fahrerwertung!C15:D15)</f>
@@ -13044,7 +13125,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:22">
       <c r="A14" s="5" t="s">
         <v>11</v>
       </c>
@@ -13054,86 +13135,86 @@
       </c>
       <c r="C14">
         <f>SUM(Fahrerwertung!C16:D16)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D14">
         <f>SUM(Fahrerwertung!C16:E16)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E14">
         <f>SUM(Fahrerwertung!C16:F16)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F14">
         <f>SUM(Fahrerwertung!C16:G16)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G14">
         <f>SUM(Fahrerwertung!C16:H16)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H14">
         <f>SUM(Fahrerwertung!C16:I16)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I14">
         <f>SUM(Fahrerwertung!C16:J16)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J14">
         <f>SUM(Fahrerwertung!C16:K16)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K14">
         <f>SUM(Fahrerwertung!C16:L16)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L14">
         <f>SUM(Fahrerwertung!C16:M16)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M14">
         <f>SUM(Fahrerwertung!C16:N16)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N14">
         <f>SUM(Fahrerwertung!C16:O16)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O14">
         <f>SUM(Fahrerwertung!C16:P16)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P14">
         <f>SUM(Fahrerwertung!C16:Q16)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q14">
         <f>SUM(Fahrerwertung!C16:R16)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R14">
         <f>SUM(Fahrerwertung!C16:S16)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S14">
         <f>SUM(Fahrerwertung!C16:T16)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T14">
         <f>SUM(Fahrerwertung!C16:U16)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U14">
         <f>SUM(Fahrerwertung!C16:V16)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V14">
         <f>SUM(Fahrerwertung!C16:W16)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:22">
       <c r="A15" s="4" t="s">
         <v>57</v>
       </c>
@@ -13147,82 +13228,82 @@
       </c>
       <c r="D15">
         <f>SUM(Fahrerwertung!C17:E17)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E15">
         <f>SUM(Fahrerwertung!C17:F17)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F15">
         <f>SUM(Fahrerwertung!C17:G17)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G15">
         <f>SUM(Fahrerwertung!C17:H17)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H15">
         <f>SUM(Fahrerwertung!C17:I17)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I15">
         <f>SUM(Fahrerwertung!C17:J17)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J15">
         <f>SUM(Fahrerwertung!C17:K17)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K15">
         <f>SUM(Fahrerwertung!C17:L17)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L15">
         <f>SUM(Fahrerwertung!C17:M17)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M15">
         <f>SUM(Fahrerwertung!C17:N17)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N15">
         <f>SUM(Fahrerwertung!C17:O17)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O15">
         <f>SUM(Fahrerwertung!C17:P17)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P15">
         <f>SUM(Fahrerwertung!C17:Q17)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q15">
         <f>SUM(Fahrerwertung!C17:R17)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R15">
         <f>SUM(Fahrerwertung!C17:S17)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S15">
         <f>SUM(Fahrerwertung!C17:T17)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T15">
         <f>SUM(Fahrerwertung!C17:U17)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U15">
         <f>SUM(Fahrerwertung!C17:V17)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V15">
         <f>SUM(Fahrerwertung!C17:W17)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:22">
       <c r="A16" s="4" t="s">
         <v>9</v>
       </c>
@@ -13311,7 +13392,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:22">
       <c r="A17" s="8" t="s">
         <v>14</v>
       </c>
@@ -13400,7 +13481,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:22">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -13489,7 +13570,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:22">
       <c r="A19" s="7" t="s">
         <v>18</v>
       </c>
@@ -13578,7 +13659,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:22">
       <c r="A20" t="s">
         <v>16</v>
       </c>
@@ -13667,7 +13748,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:22">
       <c r="A21" s="1" t="s">
         <v>2</v>
       </c>

</xml_diff>